<commit_message>
Specifying Ant. krill in species params
</commit_message>
<xml_diff>
--- a/excel data/zoop_parameters_v1.xlsx
+++ b/excel data/zoop_parameters_v1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26529"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universitytasmania-my.sharepoint.com/personal/kieran_murphy_utas_edu_au/Documents/Documents/R Projects/MFSO/excel data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universitytasmania-my.sharepoint.com/personal/kieran_murphy_utas_edu_au/Documents/Documents/R Projects/Prydz_Bay_mizer/excel data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{ECCCC34C-2F2F-2047-BD1F-2191CC419BC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FDAC970B-9C1F-4F35-80D6-DD5E579C833E}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="38700" windowHeight="15885" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="zooplankton" sheetId="1" r:id="rId1"/>
@@ -1652,7 +1652,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1661,29 +1661,27 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2033,2522 +2031,2522 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H170"/>
   <sheetViews>
-    <sheetView topLeftCell="A72" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A69" sqref="A69"/>
-      <selection pane="topRight" activeCell="C88" sqref="C88"/>
+      <selection pane="topRight" activeCell="D94" sqref="D94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.125" style="8" customWidth="1"/>
-    <col min="2" max="2" width="39.125" style="8" customWidth="1"/>
-    <col min="3" max="4" width="34.375" style="9" customWidth="1"/>
-    <col min="5" max="5" width="38.625" style="8" customWidth="1"/>
-    <col min="6" max="6" width="36" style="8" customWidth="1"/>
-    <col min="7" max="16384" width="11.125" style="8"/>
+    <col min="1" max="1" width="23.125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="39.125" style="2" customWidth="1"/>
+    <col min="3" max="4" width="34.375" style="7" customWidth="1"/>
+    <col min="5" max="5" width="38.625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="36" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="11.125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>355</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="7">
         <f>(0.07+ 0.13)/2</f>
         <v>0.1</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="7" t="s">
         <v>358</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="2" t="s">
         <v>356</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="7">
         <v>75.8</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="7" t="s">
         <v>360</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="2" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="7">
         <v>0</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="7" t="s">
         <v>361</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="28.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="7">
         <v>3700</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="7" t="s">
         <v>361</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="2" t="s">
         <v>362</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="2" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="7">
         <v>250</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="7" t="s">
         <v>363</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="2" t="s">
         <v>364</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="7">
         <v>30</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="7" t="s">
         <v>365</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="2" t="s">
         <v>366</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="7" t="s">
         <v>323</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F12" s="2" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="F14" s="6"/>
+      <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="10" t="s">
+      <c r="D15" s="2"/>
+      <c r="E15" s="8" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="7" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E17" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="7" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="F19" s="2" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E20" s="2" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="F21" s="8" t="s">
+      <c r="F21" s="2" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E22" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="F22" s="8" t="s">
+      <c r="F22" s="2" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="D23" s="11"/>
-      <c r="E23" s="10" t="s">
+      <c r="D23" s="9"/>
+      <c r="E23" s="8" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="E24" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="F24" s="8" t="s">
+      <c r="F24" s="2" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="25" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="6" t="s">
+    <row r="25" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-    </row>
-    <row r="26" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="6" t="s">
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C26" s="7" t="s">
         <v>350</v>
       </c>
-      <c r="D26" s="9"/>
-      <c r="E26" s="8" t="s">
+      <c r="D26" s="7"/>
+      <c r="E26" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="F26" s="8" t="s">
+      <c r="F26" s="2" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="6" t="s">
+    <row r="27" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="B27" s="8"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
     </row>
     <row r="28" spans="1:6" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="C30" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8" t="s">
+      <c r="D30" s="2"/>
+      <c r="E30" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="F30" s="8" t="s">
+      <c r="F30" s="2" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="C31" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8" t="s">
+      <c r="D31" s="2"/>
+      <c r="E31" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="F31" s="8" t="s">
+      <c r="F31" s="2" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8" t="s">
+      <c r="D32" s="2"/>
+      <c r="E32" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="F32" s="8" t="s">
+      <c r="F32" s="2" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="6" t="s">
+      <c r="A33" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
     </row>
     <row r="34" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="C34" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8" t="s">
+      <c r="D34" s="2"/>
+      <c r="E34" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="F34" s="8" t="s">
+      <c r="F34" s="2" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="6" t="s">
+      <c r="A35" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C35" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8" t="s">
+      <c r="D35" s="2"/>
+      <c r="E35" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="F35" s="8" t="s">
+      <c r="F35" s="2" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="6" t="s">
+      <c r="A36" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B36" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C36" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8" t="s">
+      <c r="D36" s="2"/>
+      <c r="E36" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F36" s="8" t="s">
+      <c r="F36" s="2" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="6" t="s">
+      <c r="A37" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="C37" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8" t="s">
+      <c r="D37" s="2"/>
+      <c r="E37" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="F37" s="8" t="s">
+      <c r="F37" s="2" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="6" t="s">
+      <c r="A38" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="B38" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C38" s="8" t="s">
+      <c r="C38" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8" t="s">
+      <c r="D38" s="2"/>
+      <c r="E38" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F38" s="8" t="s">
+      <c r="F38" s="2" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="6" t="s">
+      <c r="A39" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="C39" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8" t="s">
+      <c r="D39" s="2"/>
+      <c r="E39" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="F39" s="8" t="s">
+      <c r="F39" s="2" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="40" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="6" t="s">
+    <row r="40" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="B40" s="8"/>
-      <c r="C40" s="8" t="s">
+      <c r="B40" s="2"/>
+      <c r="C40" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8" t="s">
+      <c r="D40" s="2"/>
+      <c r="E40" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="F40" s="8" t="s">
+      <c r="F40" s="2" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="6" t="s">
+      <c r="A41" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="B41" s="8" t="s">
+      <c r="B41" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C41" s="8" t="s">
+      <c r="C41" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8" t="s">
+      <c r="D41" s="2"/>
+      <c r="E41" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="F41" s="8" t="s">
+      <c r="F41" s="2" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="6" t="s">
+      <c r="A42" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C42" s="8" t="s">
+      <c r="C42" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8" t="s">
+      <c r="D42" s="2"/>
+      <c r="E42" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="F42" s="8" t="s">
+      <c r="F42" s="2" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="6" t="s">
+      <c r="A43" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C43" s="8" t="s">
+      <c r="C43" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="D43" s="8"/>
-      <c r="E43" s="8" t="s">
+      <c r="D43" s="2"/>
+      <c r="E43" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="F43" s="8" t="s">
+      <c r="F43" s="2" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="6" t="s">
+      <c r="A44" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C44" s="8" t="s">
+      <c r="C44" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="D44" s="8"/>
-      <c r="E44" s="8" t="s">
+      <c r="D44" s="2"/>
+      <c r="E44" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="F44" s="8" t="s">
+      <c r="F44" s="2" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="6" t="s">
+      <c r="A45" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="B45" s="8" t="s">
+      <c r="B45" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C45" s="8"/>
-      <c r="D45" s="8"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" s="6" t="s">
+      <c r="A46" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="B46" s="8" t="s">
+      <c r="B46" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C46" s="8"/>
-      <c r="D46" s="8"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" s="6" t="s">
+      <c r="A47" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="B47" s="8" t="s">
+      <c r="B47" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="C47" s="8" t="s">
+      <c r="C47" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="D47" s="8"/>
-      <c r="E47" s="8" t="s">
+      <c r="D47" s="2"/>
+      <c r="E47" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="F47" s="8" t="s">
+      <c r="F47" s="2" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="6" t="s">
+      <c r="A49" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B49" s="8" t="s">
+      <c r="B49" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C49" s="9" t="s">
+      <c r="C49" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="E49" s="8" t="s">
+      <c r="E49" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="F49" s="8" t="s">
+      <c r="F49" s="2" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="6" t="s">
+      <c r="A50" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B50" s="8" t="s">
+      <c r="B50" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C50" s="9" t="s">
+      <c r="C50" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="E50" s="8" t="s">
+      <c r="E50" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="F50" s="8" t="s">
+      <c r="F50" s="2" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="51" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="6" t="s">
+    <row r="51" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B51" s="8" t="s">
+      <c r="B51" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C51" s="9" t="s">
+      <c r="C51" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D51" s="9"/>
-      <c r="E51" s="8"/>
-      <c r="F51" s="8"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" s="6" t="s">
+      <c r="A52" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B52" s="8" t="s">
+      <c r="B52" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C52" s="9" t="s">
+      <c r="C52" s="7" t="s">
         <v>221</v>
       </c>
-      <c r="E52" s="8" t="s">
+      <c r="E52" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="F52" s="8" t="s">
+      <c r="F52" s="2" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" s="6" t="s">
+      <c r="A53" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B53" s="8" t="s">
+      <c r="B53" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C53" s="9" t="s">
+      <c r="C53" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="E53" s="8" t="s">
+      <c r="E53" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="F53" s="8" t="s">
+      <c r="F53" s="2" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" s="6" t="s">
+      <c r="A54" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B54" s="8" t="s">
+      <c r="B54" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55" s="6" t="s">
+      <c r="A55" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B55" s="8" t="s">
+      <c r="B55" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C55" s="9" t="s">
+      <c r="C55" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="E55" s="8" t="s">
+      <c r="E55" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="F55" s="8" t="s">
+      <c r="F55" s="2" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A56" s="6" t="s">
+      <c r="A56" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B56" s="8" t="s">
+      <c r="B56" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A57" s="6" t="s">
+      <c r="A57" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B57" s="8" t="s">
+      <c r="B57" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C57" s="9" t="s">
+      <c r="C57" s="7" t="s">
         <v>226</v>
       </c>
-      <c r="E57" s="8" t="s">
+      <c r="E57" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="F57" s="8" t="s">
+      <c r="F57" s="2" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58" s="6" t="s">
+      <c r="A58" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B58" s="8" t="s">
+      <c r="B58" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C58" s="9" t="s">
+      <c r="C58" s="7" t="s">
         <v>263</v>
       </c>
-      <c r="E58" s="8" t="s">
+      <c r="E58" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="F58" s="8" t="s">
+      <c r="F58" s="2" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59" s="6" t="s">
+      <c r="A59" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B59" s="8" t="s">
+      <c r="B59" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C59" s="9" t="s">
+      <c r="C59" s="7" t="s">
         <v>266</v>
       </c>
-      <c r="E59" s="8" t="s">
+      <c r="E59" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="F59" s="8" t="s">
+      <c r="F59" s="2" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60" s="6" t="s">
+      <c r="A60" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B60" s="8" t="s">
+      <c r="B60" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="C60" s="9" t="s">
+      <c r="C60" s="7" t="s">
         <v>268</v>
       </c>
-      <c r="E60" s="8" t="s">
+      <c r="E60" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="F60" s="8" t="s">
+      <c r="F60" s="2" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A61" s="6" t="s">
+      <c r="A61" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B61" s="8" t="s">
+      <c r="B61" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="C61" s="8" t="s">
+      <c r="C61" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="D61" s="8"/>
-      <c r="E61" s="8" t="s">
+      <c r="D61" s="2"/>
+      <c r="E61" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="F61" s="8" t="s">
+      <c r="F61" s="2" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A63" s="6" t="s">
+      <c r="A63" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B63" s="6" t="s">
+      <c r="B63" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="C63" s="9" t="s">
+      <c r="C63" s="7" t="s">
         <v>299</v>
       </c>
-      <c r="E63" s="8" t="s">
+      <c r="E63" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="F63" s="8" t="s">
+      <c r="F63" s="2" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A64" s="6" t="s">
+      <c r="A64" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B64" s="8" t="s">
+      <c r="B64" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C64" s="9" t="s">
+      <c r="C64" s="7" t="s">
         <v>301</v>
       </c>
-      <c r="E64" s="8" t="s">
+      <c r="E64" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="F64" s="8" t="s">
+      <c r="F64" s="2" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="65" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="6" t="s">
+    <row r="65" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B65" s="8" t="s">
+      <c r="B65" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C65" s="9" t="s">
+      <c r="C65" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D65" s="9"/>
-      <c r="E65" s="8"/>
-      <c r="F65" s="8"/>
+      <c r="D65" s="7"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
     </row>
     <row r="66" spans="1:6" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="6" t="s">
+      <c r="A66" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B66" s="8" t="s">
+      <c r="B66" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C66" s="9" t="s">
+      <c r="C66" s="7" t="s">
         <v>307</v>
       </c>
-      <c r="E66" s="8" t="s">
+      <c r="E66" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="F66" s="8" t="s">
+      <c r="F66" s="2" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67" s="6" t="s">
+      <c r="A67" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B67" s="8" t="s">
+      <c r="B67" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C67" s="9" t="s">
+      <c r="C67" s="7" t="s">
         <v>302</v>
       </c>
-      <c r="E67" s="8" t="s">
+      <c r="E67" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="F67" s="8" t="s">
+      <c r="F67" s="2" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A68" s="6" t="s">
+      <c r="A68" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B68" s="8" t="s">
+      <c r="B68" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C68" s="9" t="s">
+      <c r="C68" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="E68" s="8" t="s">
+      <c r="E68" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="F68" s="8" t="s">
+      <c r="F68" s="2" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A69" s="6" t="s">
+      <c r="A69" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B69" s="8" t="s">
+      <c r="B69" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C69" s="9" t="s">
+      <c r="C69" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="E69" s="8" t="s">
+      <c r="E69" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="F69" s="8" t="s">
+      <c r="F69" s="2" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A70" s="6" t="s">
+      <c r="A70" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B70" s="8" t="s">
+      <c r="B70" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C70" s="9" t="s">
+      <c r="C70" s="7" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A71" s="6" t="s">
+      <c r="A71" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B71" s="8" t="s">
+      <c r="B71" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C71" s="9" t="s">
+      <c r="C71" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="E71" s="8" t="s">
+      <c r="E71" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="F71" s="8" t="s">
+      <c r="F71" s="2" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A72" s="6" t="s">
+      <c r="A72" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B72" s="8" t="s">
+      <c r="B72" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C72" s="9" t="s">
+      <c r="C72" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="E72" s="8" t="s">
+      <c r="E72" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F72" s="8" t="s">
+      <c r="F72" s="2" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A73" s="6" t="s">
+      <c r="A73" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B73" s="8" t="s">
+      <c r="B73" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C73" s="9" t="s">
+      <c r="C73" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="E73" s="8" t="s">
+      <c r="E73" s="2" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A74" s="6" t="s">
+      <c r="A74" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B74" s="8" t="s">
+      <c r="B74" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A75" s="6" t="s">
+      <c r="A75" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B75" s="8" t="s">
+      <c r="B75" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="C75" s="9" t="s">
+      <c r="C75" s="7" t="s">
         <v>311</v>
       </c>
-      <c r="E75" s="8" t="s">
+      <c r="E75" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="F75" s="8" t="s">
+      <c r="F75" s="2" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A77" s="6" t="s">
+      <c r="A77" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B77" s="6" t="s">
+      <c r="B77" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C77" s="7" t="s">
+      <c r="C77" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D77" s="7"/>
-      <c r="E77" s="6" t="s">
+      <c r="D77" s="6"/>
+      <c r="E77" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F77" s="6" t="s">
+      <c r="F77" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A78" s="6" t="s">
+      <c r="A78" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B78" s="8" t="s">
+      <c r="B78" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C78" s="9" t="s">
+      <c r="C78" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E78" s="8" t="s">
+      <c r="E78" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F78" s="10" t="s">
+      <c r="F78" s="8" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A79" s="6" t="s">
+      <c r="A79" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B79" s="8" t="s">
+      <c r="B79" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="80" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="6" t="s">
+    <row r="80" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B80" s="8" t="s">
+      <c r="B80" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C80" s="9" t="s">
+      <c r="C80" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D80" s="9"/>
-      <c r="E80" s="8" t="s">
+      <c r="D80" s="7"/>
+      <c r="E80" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F80" s="8"/>
+      <c r="F80" s="2"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A81" s="6" t="s">
+      <c r="A81" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B81" s="8" t="s">
+      <c r="B81" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C81" s="9" t="s">
+      <c r="C81" s="7" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A82" s="6" t="s">
+      <c r="A82" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B82" s="8" t="s">
+      <c r="B82" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C82" s="9" t="s">
+      <c r="C82" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E82" s="8" t="s">
+      <c r="E82" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F82" s="8" t="s">
+      <c r="F82" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A83" s="6" t="s">
+      <c r="A83" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B83" s="8" t="s">
+      <c r="B83" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C83" s="9" t="s">
+      <c r="C83" s="7" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A84" s="6" t="s">
+      <c r="A84" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B84" s="8" t="s">
+      <c r="B84" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C84" s="9" t="s">
+      <c r="C84" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="E84" s="8" t="s">
+      <c r="E84" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A85" s="6" t="s">
+      <c r="A85" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B85" s="8" t="s">
+      <c r="B85" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C85" s="9" t="s">
+      <c r="C85" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E85" s="8" t="s">
+      <c r="E85" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F85" s="8" t="s">
+      <c r="F85" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A86" s="6" t="s">
+      <c r="A86" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B86" s="8" t="s">
+      <c r="B86" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C86" s="9" t="s">
+      <c r="C86" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E86" s="8" t="s">
+      <c r="E86" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F86" s="8" t="s">
+      <c r="F86" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A87" s="6" t="s">
+      <c r="A87" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B87" s="8" t="s">
+      <c r="B87" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C87" s="9" t="s">
+      <c r="C87" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="E87" s="8" t="s">
+      <c r="E87" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F87" s="8" t="s">
+      <c r="F87" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A88" s="6" t="s">
+      <c r="A88" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B88" s="8" t="s">
+      <c r="B88" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C88" s="9" t="s">
+      <c r="C88" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="E88" s="8" t="s">
+      <c r="E88" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F88" s="10" t="s">
+      <c r="F88" s="8" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A89" s="6" t="s">
+      <c r="A89" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B89" s="8" t="s">
+      <c r="B89" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C89" s="9" t="s">
+      <c r="C89" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="E89" s="8" t="s">
+      <c r="E89" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F89" s="8" t="s">
+      <c r="F89" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A90" s="6" t="s">
+      <c r="A90" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B90" s="8" t="s">
+      <c r="B90" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A91" s="6" t="s">
+      <c r="A91" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B91" s="8" t="s">
+      <c r="B91" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="C91" s="9" t="s">
+      <c r="C91" s="7" t="s">
         <v>320</v>
       </c>
-      <c r="E91" s="8" t="s">
+      <c r="E91" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="F91" s="8" t="s">
+      <c r="F91" s="2" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A93" s="6" t="s">
+      <c r="A93" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B93" s="6" t="s">
+      <c r="B93" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C93" s="7" t="s">
+      <c r="C93" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="D93" s="7"/>
-      <c r="E93" s="8" t="s">
+      <c r="D93" s="6"/>
+      <c r="E93" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="F93" s="6" t="s">
+      <c r="F93" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="94" spans="1:6" s="6" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="6" t="s">
+    <row r="94" spans="1:6" s="1" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B94" s="8" t="s">
+      <c r="B94" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C94" s="9"/>
-      <c r="D94" s="9"/>
-      <c r="E94" s="8"/>
-      <c r="F94" s="10" t="s">
+      <c r="C94" s="7"/>
+      <c r="D94" s="7"/>
+      <c r="E94" s="2"/>
+      <c r="F94" s="8" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A95" s="6" t="s">
+      <c r="A95" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B95" s="8" t="s">
+      <c r="B95" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C95" s="9" t="s">
+      <c r="C95" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E95" s="8" t="s">
+      <c r="E95" s="2" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A96" s="6" t="s">
+      <c r="A96" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B96" s="8" t="s">
+      <c r="B96" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C96" s="9" t="s">
+      <c r="C96" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="E96" s="8" t="s">
+      <c r="E96" s="2" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A97" s="6" t="s">
+      <c r="A97" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B97" s="8" t="s">
+      <c r="B97" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C97" s="9" t="s">
+      <c r="C97" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="E97" s="8" t="s">
+      <c r="E97" s="2" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A98" s="6" t="s">
+      <c r="A98" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B98" s="8" t="s">
+      <c r="B98" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C98" s="9" t="s">
+      <c r="C98" s="7" t="s">
         <v>274</v>
       </c>
-      <c r="E98" s="8" t="s">
+      <c r="E98" s="2" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A99" s="6" t="s">
+      <c r="A99" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B99" s="8" t="s">
+      <c r="B99" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C99" s="9" t="s">
+      <c r="C99" s="7" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A100" s="6" t="s">
+      <c r="A100" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B100" s="8" t="s">
+      <c r="B100" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C100" s="9">
+      <c r="C100" s="7">
         <v>0.5</v>
       </c>
-      <c r="E100" s="8" t="s">
+      <c r="E100" s="2" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A101" s="6" t="s">
+      <c r="A101" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B101" s="8" t="s">
+      <c r="B101" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C101" s="9" t="s">
+      <c r="C101" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="E101" s="8" t="s">
+      <c r="E101" s="2" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A102" s="6" t="s">
+      <c r="A102" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B102" s="8" t="s">
+      <c r="B102" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C102" s="9" t="s">
+      <c r="C102" s="7" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A103" s="6" t="s">
+      <c r="A103" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B103" s="8" t="s">
+      <c r="B103" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A104" s="6" t="s">
+      <c r="A104" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B104" s="8" t="s">
+      <c r="B104" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A105" s="6" t="s">
+      <c r="A105" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B105" s="8" t="s">
+      <c r="B105" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="C105" s="9" t="s">
+      <c r="C105" s="7" t="s">
         <v>327</v>
       </c>
-      <c r="E105" s="8" t="s">
+      <c r="E105" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="F105" s="8" t="s">
+      <c r="F105" s="2" t="s">
         <v>329</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B107" s="6" t="s">
+      <c r="B107" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C107" s="7" t="s">
+      <c r="C107" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="D107" s="7"/>
-      <c r="E107" s="6" t="s">
+      <c r="D107" s="6"/>
+      <c r="E107" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="F107" s="6" t="s">
+      <c r="F107" s="1" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A108" s="6" t="s">
+      <c r="A108" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B108" s="8" t="s">
+      <c r="B108" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C108" s="9" t="s">
+      <c r="C108" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="E108" s="8" t="s">
+      <c r="E108" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="F108" s="8" t="s">
+      <c r="F108" s="2" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A109" s="6" t="s">
+      <c r="A109" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B109" s="8" t="s">
+      <c r="B109" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C109" s="9" t="s">
+      <c r="C109" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="E109" s="8" t="s">
+      <c r="E109" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="F109" s="8" t="s">
+      <c r="F109" s="2" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A110" s="6" t="s">
+      <c r="A110" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B110" s="8" t="s">
+      <c r="B110" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C110" s="9" t="s">
+      <c r="C110" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="E110" s="8" t="s">
+      <c r="E110" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="F110" s="8" t="s">
+      <c r="F110" s="2" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A111" s="6" t="s">
+      <c r="A111" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B111" s="8" t="s">
+      <c r="B111" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C111" s="9" t="s">
+      <c r="C111" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="E111" s="8" t="s">
+      <c r="E111" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="F111" s="8" t="s">
+      <c r="F111" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="G111" s="8" t="s">
+      <c r="G111" s="2" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A112" s="6" t="s">
+      <c r="A112" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B112" s="8" t="s">
+      <c r="B112" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C112" s="9" t="s">
+      <c r="C112" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="E112" s="8" t="s">
+      <c r="E112" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="F112" s="8" t="s">
+      <c r="F112" s="2" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A113" s="6" t="s">
+      <c r="A113" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B113" s="8" t="s">
+      <c r="B113" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C113" s="9" t="s">
+      <c r="C113" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="E113" s="8" t="s">
+      <c r="E113" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="F113" s="8" t="s">
+      <c r="F113" s="2" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A114" s="6" t="s">
+      <c r="A114" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B114" s="8" t="s">
+      <c r="B114" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C114" s="9" t="s">
+      <c r="C114" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="E114" s="8" t="s">
+      <c r="E114" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="F114" s="8" t="s">
+      <c r="F114" s="2" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A115" s="6" t="s">
+      <c r="A115" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B115" s="8" t="s">
+      <c r="B115" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C115" s="9" t="s">
+      <c r="C115" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="E115" s="8" t="s">
+      <c r="E115" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="F115" s="8" t="s">
+      <c r="F115" s="2" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A116" s="6" t="s">
+      <c r="A116" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B116" s="8" t="s">
+      <c r="B116" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C116" s="9" t="s">
+      <c r="C116" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="E116" s="8" t="s">
+      <c r="E116" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="F116" s="8" t="s">
+      <c r="F116" s="2" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A117" s="6" t="s">
+      <c r="A117" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B117" s="8" t="s">
+      <c r="B117" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C117" s="9" t="s">
+      <c r="C117" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="E117" s="8" t="s">
+      <c r="E117" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="F117" s="8" t="s">
+      <c r="F117" s="2" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A118" s="6" t="s">
+      <c r="A118" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B118" s="8" t="s">
+      <c r="B118" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C118" s="9" t="s">
+      <c r="C118" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="E118" s="8" t="s">
+      <c r="E118" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="F118" s="8" t="s">
+      <c r="F118" s="2" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A119" s="6" t="s">
+      <c r="A119" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B119" s="8" t="s">
+      <c r="B119" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C119" s="9" t="s">
+      <c r="C119" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="E119" s="8" t="s">
+      <c r="E119" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="F119" s="8" t="s">
+      <c r="F119" s="2" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A120" s="6" t="s">
+      <c r="A120" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B120" s="8" t="s">
+      <c r="B120" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C120" s="9" t="s">
+      <c r="C120" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="E120" s="8" t="s">
+      <c r="E120" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="F120" s="8" t="s">
+      <c r="F120" s="2" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A121" s="6" t="s">
+      <c r="A121" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B121" s="8" t="s">
+      <c r="B121" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C121" s="9" t="s">
+      <c r="C121" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="E121" s="8" t="s">
+      <c r="E121" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="F121" s="8" t="s">
+      <c r="F121" s="2" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A122" s="6" t="s">
+      <c r="A122" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B122" s="8" t="s">
+      <c r="B122" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C122" s="9" t="s">
+      <c r="C122" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="E122" s="8" t="s">
+      <c r="E122" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="F122" s="8" t="s">
+      <c r="F122" s="2" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A123" s="6" t="s">
+      <c r="A123" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B123" s="8" t="s">
+      <c r="B123" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C123" s="9" t="s">
+      <c r="C123" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="E123" s="8" t="s">
+      <c r="E123" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="F123" s="8" t="s">
+      <c r="F123" s="2" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A124" s="6" t="s">
+      <c r="A124" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B124" s="8" t="s">
+      <c r="B124" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C124" s="9" t="s">
+      <c r="C124" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="E124" s="8" t="s">
+      <c r="E124" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="F124" s="8" t="s">
+      <c r="F124" s="2" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A125" s="6" t="s">
+      <c r="A125" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B125" s="8" t="s">
+      <c r="B125" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C125" s="9" t="s">
+      <c r="C125" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E125" s="8" t="s">
+      <c r="E125" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="F125" s="8" t="s">
+      <c r="F125" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="126" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A126" s="6" t="s">
+    <row r="126" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A126" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B126" s="8" t="s">
+      <c r="B126" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C126" s="9" t="s">
+      <c r="C126" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="D126" s="9"/>
-      <c r="E126" s="8" t="s">
+      <c r="D126" s="7"/>
+      <c r="E126" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="F126" s="8" t="s">
+      <c r="F126" s="2" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A127" s="6" t="s">
+      <c r="A127" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B127" s="8" t="s">
+      <c r="B127" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C127" s="9" t="s">
+      <c r="C127" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="E127" s="8" t="s">
+      <c r="E127" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="F127" s="8" t="s">
+      <c r="F127" s="2" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A128" s="6" t="s">
+      <c r="A128" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B128" s="8" t="s">
+      <c r="B128" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C128" s="9" t="s">
+      <c r="C128" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="E128" s="8" t="s">
+      <c r="E128" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="F128" s="8" t="s">
+      <c r="F128" s="2" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A129" s="6" t="s">
+      <c r="A129" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B129" s="8" t="s">
+      <c r="B129" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C129" s="9" t="s">
+      <c r="C129" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="E129" s="8" t="s">
+      <c r="E129" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="F129" s="8" t="s">
+      <c r="F129" s="2" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A130" s="6" t="s">
+      <c r="A130" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B130" s="8" t="s">
+      <c r="B130" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C130" s="9" t="s">
+      <c r="C130" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="E130" s="8" t="s">
+      <c r="E130" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="F130" s="8" t="s">
+      <c r="F130" s="2" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="131" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A131" s="6" t="s">
+      <c r="A131" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B131" s="8" t="s">
+      <c r="B131" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C131" s="9" t="s">
+      <c r="C131" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="E131" s="10" t="s">
+      <c r="E131" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="F131" s="8" t="s">
+      <c r="F131" s="2" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A132" s="6" t="s">
+      <c r="A132" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B132" s="8" t="s">
+      <c r="B132" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C132" s="9" t="s">
+      <c r="C132" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="E132" s="8" t="s">
+      <c r="E132" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="F132" s="8" t="s">
+      <c r="F132" s="2" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A133" s="6" t="s">
+      <c r="A133" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B133" s="8" t="s">
+      <c r="B133" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C133" s="9" t="s">
+      <c r="C133" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="E133" s="8" t="s">
+      <c r="E133" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="F133" s="8" t="s">
+      <c r="F133" s="2" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="134" spans="1:8" s="10" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A134" s="6" t="s">
+    <row r="134" spans="1:8" s="8" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A134" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B134" s="8" t="s">
+      <c r="B134" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C134" s="9"/>
-      <c r="D134" s="9"/>
-      <c r="E134" s="8"/>
-      <c r="F134" s="8"/>
+      <c r="C134" s="7"/>
+      <c r="D134" s="7"/>
+      <c r="E134" s="2"/>
+      <c r="F134" s="2"/>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A135" s="6" t="s">
+      <c r="A135" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B135" s="8" t="s">
+      <c r="B135" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="C135" s="9" t="s">
+      <c r="C135" s="7" t="s">
         <v>354</v>
       </c>
-      <c r="E135" s="8" t="s">
+      <c r="E135" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="F135" s="8" t="s">
+      <c r="F135" s="2" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A136" s="6"/>
+      <c r="A136" s="1"/>
     </row>
     <row r="137" spans="1:8" ht="53.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A137" s="6" t="s">
+      <c r="A137" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B137" s="6" t="s">
+      <c r="B137" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C137" s="7"/>
-      <c r="D137" s="7"/>
-      <c r="E137" s="6"/>
-      <c r="F137" s="13" t="s">
+      <c r="C137" s="6"/>
+      <c r="D137" s="6"/>
+      <c r="E137" s="1"/>
+      <c r="F137" s="11" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A138" s="6" t="s">
+      <c r="A138" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B138" s="8" t="s">
+      <c r="B138" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="139" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A139" s="6" t="s">
+    <row r="139" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A139" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B139" s="8" t="s">
+      <c r="B139" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C139" s="9"/>
-      <c r="D139" s="9"/>
-      <c r="E139" s="8"/>
-      <c r="F139" s="8"/>
-      <c r="H139" s="8"/>
+      <c r="C139" s="7"/>
+      <c r="D139" s="7"/>
+      <c r="E139" s="2"/>
+      <c r="F139" s="2"/>
+      <c r="H139" s="2"/>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A140" s="6" t="s">
+      <c r="A140" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B140" s="8" t="s">
+      <c r="B140" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A141" s="6" t="s">
+      <c r="A141" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B141" s="8" t="s">
+      <c r="B141" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C141" s="9" t="s">
+      <c r="C141" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="E141" s="8" t="s">
+      <c r="E141" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="F141" s="8" t="s">
+      <c r="F141" s="2" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A142" s="6" t="s">
+      <c r="A142" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B142" s="8" t="s">
+      <c r="B142" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A143" s="6" t="s">
+      <c r="A143" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B143" s="8" t="s">
+      <c r="B143" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C143" s="2" t="s">
         <v>206</v>
       </c>
       <c r="D143" s="2"/>
-      <c r="E143" s="8" t="s">
+      <c r="E143" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="F143" s="8" t="s">
+      <c r="F143" s="2" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A144" s="6" t="s">
+      <c r="A144" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B144" s="8" t="s">
+      <c r="B144" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="145" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A145" s="6" t="s">
+      <c r="A145" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B145" s="10" t="s">
+      <c r="B145" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C145" s="11" t="s">
+      <c r="C145" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="D145" s="11"/>
-      <c r="E145" s="10" t="s">
+      <c r="D145" s="9"/>
+      <c r="E145" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="F145" s="10" t="s">
+      <c r="F145" s="8" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A146" s="6" t="s">
+      <c r="A146" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B146" s="8" t="s">
+      <c r="B146" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C146" s="9" t="s">
+      <c r="C146" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="E146" s="8" t="s">
+      <c r="E146" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="F146" s="8" t="s">
+      <c r="F146" s="2" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A147" s="6" t="s">
+      <c r="A147" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B147" s="8" t="s">
+      <c r="B147" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A148" s="6" t="s">
+      <c r="A148" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B148" s="8" t="s">
+      <c r="B148" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A149" s="6" t="s">
+      <c r="A149" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B149" s="8" t="s">
+      <c r="B149" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="C149" s="9" t="s">
+      <c r="C149" s="7" t="s">
         <v>346</v>
       </c>
-      <c r="E149" s="8" t="s">
+      <c r="E149" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="F149" s="8" t="s">
+      <c r="F149" s="2" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A150" s="6" t="s">
+      <c r="A150" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A151" s="6" t="s">
+      <c r="A151" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B151" s="8" t="s">
+      <c r="B151" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C151" s="12" t="s">
+      <c r="C151" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="D151" s="12"/>
-      <c r="E151" s="8" t="s">
+      <c r="D151" s="10"/>
+      <c r="E151" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="F151" s="8" t="s">
+      <c r="F151" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="G151" s="8" t="s">
+      <c r="G151" s="2" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A152" s="6" t="s">
+      <c r="A152" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B152" s="8" t="s">
+      <c r="B152" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C152" s="12" t="s">
+      <c r="C152" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="D152" s="12"/>
-      <c r="E152" s="8" t="s">
+      <c r="D152" s="10"/>
+      <c r="E152" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="F152" s="8" t="s">
+      <c r="F152" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="G152" s="8" t="s">
+      <c r="G152" s="2" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="153" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A153" s="6" t="s">
+      <c r="A153" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B153" s="8" t="s">
+      <c r="B153" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C153" s="12" t="s">
+      <c r="C153" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="D153" s="12"/>
-      <c r="E153" s="8" t="s">
+      <c r="D153" s="10"/>
+      <c r="E153" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="F153" s="10" t="s">
+      <c r="F153" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="G153" s="8" t="s">
+      <c r="G153" s="2" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="154" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A154" s="6" t="s">
+      <c r="A154" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B154" s="8" t="s">
+      <c r="B154" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C154" s="12" t="s">
+      <c r="C154" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="D154" s="12"/>
-      <c r="E154" s="8" t="s">
+      <c r="D154" s="10"/>
+      <c r="E154" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="F154" s="10" t="s">
+      <c r="F154" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="G154" s="8" t="s">
+      <c r="G154" s="2" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="155" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A155" s="6" t="s">
+      <c r="A155" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B155" s="8" t="s">
+      <c r="B155" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C155" s="12" t="s">
+      <c r="C155" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="D155" s="12"/>
-      <c r="E155" s="8" t="s">
+      <c r="D155" s="10"/>
+      <c r="E155" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="F155" s="10" t="s">
+      <c r="F155" s="8" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A156" s="6" t="s">
+      <c r="A156" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B156" s="8" t="s">
+      <c r="B156" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C156" s="12" t="s">
+      <c r="C156" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="D156" s="12"/>
-      <c r="E156" s="8" t="s">
+      <c r="D156" s="10"/>
+      <c r="E156" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="F156" s="8" t="s">
+      <c r="F156" s="2" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A157" s="6" t="s">
+      <c r="A157" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B157" s="8" t="s">
+      <c r="B157" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C157" s="8" t="s">
+      <c r="C157" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="D157" s="8"/>
-      <c r="E157" s="8" t="s">
+      <c r="D157" s="2"/>
+      <c r="E157" s="2" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A158" s="6" t="s">
+      <c r="A158" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B158" s="8" t="s">
+      <c r="B158" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C158" s="8" t="s">
+      <c r="C158" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="D158" s="8"/>
-      <c r="E158" s="8" t="s">
+      <c r="D158" s="2"/>
+      <c r="E158" s="2" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A159" s="6" t="s">
+      <c r="A159" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B159" s="8" t="s">
+      <c r="B159" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C159" s="12" t="s">
+      <c r="C159" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="D159" s="12"/>
-      <c r="E159" s="8" t="s">
+      <c r="D159" s="10"/>
+      <c r="E159" s="2" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A160" s="6" t="s">
+      <c r="A160" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B160" s="8" t="s">
+      <c r="B160" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C160" s="12" t="s">
+      <c r="C160" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="D160" s="12"/>
-      <c r="E160" s="8" t="s">
+      <c r="D160" s="10"/>
+      <c r="E160" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="F160" s="8" t="s">
+      <c r="F160" s="2" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A161" s="6" t="s">
+      <c r="A161" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B161" s="8" t="s">
+      <c r="B161" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C161" s="12" t="s">
+      <c r="C161" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="D161" s="12"/>
-      <c r="E161" s="8" t="s">
+      <c r="D161" s="10"/>
+      <c r="E161" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="F161" s="8" t="s">
+      <c r="F161" s="2" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A162" s="6" t="s">
+      <c r="A162" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B162" s="8" t="s">
+      <c r="B162" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C162" s="8" t="s">
+      <c r="C162" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="D162" s="8"/>
-      <c r="E162" s="8" t="s">
+      <c r="D162" s="2"/>
+      <c r="E162" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="F162" s="8" t="s">
+      <c r="F162" s="2" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A163" s="6" t="s">
+      <c r="A163" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B163" s="8" t="s">
+      <c r="B163" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C163" s="8" t="s">
+      <c r="C163" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="D163" s="8"/>
-      <c r="E163" s="8" t="s">
+      <c r="D163" s="2"/>
+      <c r="E163" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="F163" s="8" t="s">
+      <c r="F163" s="2" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A164" s="6" t="s">
+      <c r="A164" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B164" s="8" t="s">
+      <c r="B164" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C164" s="8" t="s">
+      <c r="C164" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="D164" s="8"/>
-      <c r="E164" s="8" t="s">
+      <c r="D164" s="2"/>
+      <c r="E164" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="F164" s="8" t="s">
+      <c r="F164" s="2" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A165" s="6" t="s">
+      <c r="A165" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B165" s="8" t="s">
+      <c r="B165" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C165" s="8" t="s">
+      <c r="C165" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="D165" s="8"/>
-      <c r="E165" s="8" t="s">
+      <c r="D165" s="2"/>
+      <c r="E165" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="F165" s="8" t="s">
+      <c r="F165" s="2" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A166" s="6" t="s">
+      <c r="A166" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B166" s="8" t="s">
+      <c r="B166" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C166" s="8" t="s">
+      <c r="C166" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="D166" s="8"/>
-      <c r="E166" s="8" t="s">
+      <c r="D166" s="2"/>
+      <c r="E166" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="F166" s="8" t="s">
+      <c r="F166" s="2" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A167" s="6" t="s">
+      <c r="A167" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B167" s="8" t="s">
+      <c r="B167" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C167" s="8" t="s">
+      <c r="C167" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="D167" s="8"/>
-      <c r="E167" s="8" t="s">
+      <c r="D167" s="2"/>
+      <c r="E167" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="F167" s="8" t="s">
+      <c r="F167" s="2" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A168" s="6" t="s">
+      <c r="A168" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B168" s="8" t="s">
+      <c r="B168" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C168" s="8"/>
-      <c r="D168" s="8"/>
+      <c r="C168" s="2"/>
+      <c r="D168" s="2"/>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A169" s="6" t="s">
+      <c r="A169" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B169" s="8" t="s">
+      <c r="B169" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C169" s="8"/>
-      <c r="D169" s="8"/>
+      <c r="C169" s="2"/>
+      <c r="D169" s="2"/>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A170" s="6" t="s">
+      <c r="A170" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B170" s="8" t="s">
+      <c r="B170" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="C170" s="9" t="s">
+      <c r="C170" s="7" t="s">
         <v>331</v>
       </c>
-      <c r="E170" s="8" t="s">
+      <c r="E170" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="F170" s="8" t="s">
+      <c r="F170" s="2" t="s">
         <v>332</v>
       </c>
     </row>
@@ -4731,7 +4729,7 @@
       <c r="B12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="12" t="s">
         <v>280</v>
       </c>
       <c r="D12" s="3" t="s">
@@ -4829,7 +4827,7 @@
       <c r="B20" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="14" t="s">
         <v>294</v>
       </c>
       <c r="D20" s="5" t="s">
@@ -4901,7 +4899,7 @@
       <c r="B26" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="15" t="s">
+      <c r="C26" s="13" t="s">
         <v>281</v>
       </c>
       <c r="D26" s="5" t="s">
@@ -5054,7 +5052,7 @@
       <c r="C42" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="D42" s="8" t="s">
+      <c r="D42" s="2" t="s">
         <v>341</v>
       </c>
       <c r="E42" s="2" t="s">
@@ -5076,7 +5074,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF6AEAFE-F531-6D45-8E53-194E5508560C}">
   <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -5095,46 +5093,46 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="15" t="s">
         <v>382</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="15" t="s">
         <v>381</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="15" t="s">
         <v>380</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="15" t="s">
         <v>379</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="15" t="s">
         <v>378</v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="G3" s="15" t="s">
         <v>386</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="15" t="s">
         <v>385</v>
       </c>
-      <c r="I3" s="17" t="s">
+      <c r="I3" s="15" t="s">
         <v>387</v>
       </c>
-      <c r="J3" s="17" t="s">
+      <c r="J3" s="15" t="s">
         <v>377</v>
       </c>
-      <c r="K3" s="17" t="s">
+      <c r="K3" s="15" t="s">
         <v>376</v>
       </c>
-      <c r="L3" s="17" t="s">
+      <c r="L3" s="15" t="s">
         <v>375</v>
       </c>
-      <c r="M3" s="17" t="s">
+      <c r="M3" s="15" t="s">
         <v>389</v>
       </c>
-      <c r="N3" s="17" t="s">
+      <c r="N3" s="15" t="s">
         <v>8</v>
       </c>
     </row>
@@ -5157,13 +5155,13 @@
       <c r="F4" t="s">
         <v>374</v>
       </c>
-      <c r="G4" s="18">
+      <c r="G4" s="16">
         <v>-4.2</v>
       </c>
-      <c r="H4" s="18">
+      <c r="H4" s="16">
         <v>0.5</v>
       </c>
-      <c r="I4" s="18">
+      <c r="I4" s="16">
         <v>-1.8</v>
       </c>
       <c r="J4">
@@ -5200,13 +5198,13 @@
       <c r="F5" t="s">
         <v>371</v>
       </c>
-      <c r="G5" s="18">
+      <c r="G5" s="16">
         <v>-4.5</v>
       </c>
-      <c r="H5" s="18">
+      <c r="H5" s="16">
         <v>1.4</v>
       </c>
-      <c r="I5" s="18">
+      <c r="I5" s="16">
         <v>-0.6</v>
       </c>
       <c r="J5">
@@ -5238,13 +5236,13 @@
       <c r="F6" t="s">
         <v>367</v>
       </c>
-      <c r="G6" s="18">
+      <c r="G6" s="16">
         <v>-5</v>
       </c>
-      <c r="H6" s="18">
+      <c r="H6" s="16">
         <v>0</v>
       </c>
-      <c r="I6" s="18">
+      <c r="I6" s="16">
         <v>-2</v>
       </c>
       <c r="J6">
@@ -5270,13 +5268,13 @@
       <c r="F7" t="s">
         <v>367</v>
       </c>
-      <c r="G7" s="18">
+      <c r="G7" s="16">
         <v>-7.5</v>
       </c>
-      <c r="H7" s="18">
+      <c r="H7" s="16">
         <v>-2.5</v>
       </c>
-      <c r="I7" s="18">
+      <c r="I7" s="16">
         <v>-4.5</v>
       </c>
       <c r="J7">
@@ -5293,20 +5291,20 @@
       <c r="A8" t="s">
         <v>390</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="G8" s="18">
+      <c r="B8" s="16"/>
+      <c r="G8" s="16">
         <v>-12.3</v>
       </c>
-      <c r="H8" s="18">
+      <c r="H8" s="16">
         <v>-6</v>
       </c>
-      <c r="I8" s="18">
+      <c r="I8" s="16">
         <v>-8</v>
       </c>
-      <c r="J8" s="18">
+      <c r="J8" s="16">
         <v>500</v>
       </c>
-      <c r="K8" s="18">
+      <c r="K8" s="16">
         <v>0</v>
       </c>
     </row>
@@ -5329,19 +5327,19 @@
       <c r="F9" t="s">
         <v>96</v>
       </c>
-      <c r="G9" s="18">
+      <c r="G9" s="16">
         <v>-3</v>
       </c>
-      <c r="H9" s="18">
+      <c r="H9" s="16">
         <v>2.6</v>
       </c>
-      <c r="I9" s="18">
+      <c r="I9" s="16">
         <v>0.6</v>
       </c>
-      <c r="J9" s="18">
+      <c r="J9" s="16">
         <v>3500</v>
       </c>
-      <c r="K9" s="18">
+      <c r="K9" s="16">
         <v>0</v>
       </c>
     </row>

</xml_diff>